<commit_message>
Added new deployment file
</commit_message>
<xml_diff>
--- a/config/Master_Test_Template_project1.xlsx
+++ b/config/Master_Test_Template_project1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A4952\PycharmProjects\april_automation_framework\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF83AE3-0E71-4D75-9741-3A83218A45D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F186870F-9BDF-4F13-AB06-72B0853C248B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,9 +167,6 @@
     <t>snowflake</t>
   </si>
   <si>
-    <t>contact_info_20240702.csv</t>
-  </si>
-  <si>
     <t>contact_info_r2b_transformation.sql</t>
   </si>
   <si>
@@ -276,6 +273,9 @@
   </si>
   <si>
     <t>ETL_AUTO.CONTACT_INFO.CONTACT_INFO_BRONZE</t>
+  </si>
+  <si>
+    <t>contact_info_20240709.csv</t>
   </si>
 </sst>
 </file>
@@ -826,10 +826,10 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -929,7 +929,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>0</v>
@@ -944,7 +944,7 @@
         <v>44</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>46</v>
@@ -994,7 +994,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>0</v>
@@ -1009,7 +1009,7 @@
         <v>44</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>46</v>
@@ -1059,7 +1059,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>0</v>
@@ -1074,7 +1074,7 @@
         <v>44</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>46</v>
@@ -1124,7 +1124,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>0</v>
@@ -1139,7 +1139,7 @@
         <v>44</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>46</v>
@@ -1189,7 +1189,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>0</v>
@@ -1204,7 +1204,7 @@
         <v>44</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>46</v>
@@ -1254,7 +1254,7 @@
         <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>0</v>
@@ -1269,7 +1269,7 @@
         <v>44</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>46</v>
@@ -1319,7 +1319,7 @@
         <v>42</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>44</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>46</v>
@@ -1378,28 +1378,28 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>46</v>
@@ -1443,28 +1443,28 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>46</v>
@@ -1508,28 +1508,28 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>46</v>
@@ -1573,28 +1573,28 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>46</v>
@@ -1638,28 +1638,28 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>46</v>
@@ -1703,28 +1703,28 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>46</v>
@@ -1768,28 +1768,28 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>46</v>
@@ -1833,28 +1833,28 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="19" t="s">
         <v>82</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>83</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>46</v>
@@ -1898,13 +1898,13 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>46</v>
@@ -1913,28 +1913,28 @@
         <v>45</v>
       </c>
       <c r="F17" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="19" t="s">
+      <c r="I17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M17" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N17" s="26" t="s">
         <v>17</v>
@@ -1946,7 +1946,7 @@
         <v>21</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R17" s="2" t="s">
         <v>27</v>
@@ -1963,13 +1963,13 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>46</v>
@@ -1978,28 +1978,28 @@
         <v>45</v>
       </c>
       <c r="F18" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="19" t="s">
+      <c r="I18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J18" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K18" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N18" s="26" t="s">
         <v>17</v>
@@ -2011,7 +2011,7 @@
         <v>21</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R18" s="2" t="s">
         <v>27</v>
@@ -2028,13 +2028,13 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>46</v>
@@ -2043,28 +2043,28 @@
         <v>45</v>
       </c>
       <c r="F19" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="19" t="s">
+      <c r="I19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N19" s="26" t="s">
         <v>17</v>
@@ -2076,7 +2076,7 @@
         <v>21</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>27</v>
@@ -2093,13 +2093,13 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>46</v>
@@ -2108,28 +2108,28 @@
         <v>45</v>
       </c>
       <c r="F20" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="19" t="s">
+      <c r="I20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J20" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M20" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N20" s="26" t="s">
         <v>17</v>
@@ -2141,7 +2141,7 @@
         <v>21</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>27</v>
@@ -2158,13 +2158,13 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>46</v>
@@ -2173,28 +2173,28 @@
         <v>45</v>
       </c>
       <c r="F21" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="19" t="s">
+      <c r="I21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N21" s="26" t="s">
         <v>17</v>
@@ -2206,7 +2206,7 @@
         <v>21</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R21" s="2" t="s">
         <v>27</v>
@@ -2223,13 +2223,13 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>46</v>
@@ -2238,28 +2238,28 @@
         <v>45</v>
       </c>
       <c r="F22" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="19" t="s">
+      <c r="I22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K22" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J22" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K22" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M22" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N22" s="26" t="s">
         <v>17</v>
@@ -2271,7 +2271,7 @@
         <v>21</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>27</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>46</v>
@@ -2303,28 +2303,28 @@
         <v>45</v>
       </c>
       <c r="F23" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="19" t="s">
+      <c r="I23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K23" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M23" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N23" s="26" t="s">
         <v>17</v>
@@ -2336,7 +2336,7 @@
         <v>21</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R23" s="2" t="s">
         <v>27</v>
@@ -2353,13 +2353,13 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>46</v>
@@ -2368,28 +2368,28 @@
         <v>45</v>
       </c>
       <c r="F24" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G24" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="19" t="s">
+      <c r="I24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K24" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M24" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N24" s="26" t="s">
         <v>17</v>
@@ -2401,7 +2401,7 @@
         <v>21</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R24" s="2" t="s">
         <v>27</v>
@@ -2418,13 +2418,13 @@
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>46</v>
@@ -2433,28 +2433,28 @@
         <v>45</v>
       </c>
       <c r="F25" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G25" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="19" t="s">
+      <c r="I25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J25" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K25" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M25" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N25" s="26" t="s">
         <v>17</v>
@@ -2466,10 +2466,10 @@
         <v>21</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S25" s="2" t="s">
         <v>27</v>
@@ -2483,13 +2483,13 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>46</v>
@@ -2498,28 +2498,28 @@
         <v>45</v>
       </c>
       <c r="F26" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="19" t="s">
+      <c r="I26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J26" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K26" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M26" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N26" s="26" t="s">
         <v>17</v>
@@ -2531,10 +2531,10 @@
         <v>21</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S26" s="2" t="s">
         <v>27</v>
@@ -2548,13 +2548,13 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>46</v>
@@ -2563,28 +2563,28 @@
         <v>45</v>
       </c>
       <c r="F27" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="19" t="s">
+      <c r="I27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K27" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M27" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N27" s="26" t="s">
         <v>17</v>
@@ -2596,10 +2596,10 @@
         <v>21</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R27" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S27" s="2" t="s">
         <v>27</v>
@@ -2613,13 +2613,13 @@
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>46</v>
@@ -2628,28 +2628,28 @@
         <v>45</v>
       </c>
       <c r="F28" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G28" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="19" t="s">
+      <c r="I28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J28" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K28" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M28" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="N28" s="26" t="s">
         <v>17</v>
@@ -2661,13 +2661,13 @@
         <v>21</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S28" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="T28" s="2">
         <v>0</v>

</xml_diff>